<commit_message>
Final run for illustration
</commit_message>
<xml_diff>
--- a/optimization_results.xlsx
+++ b/optimization_results.xlsx
@@ -23,10 +23,10 @@
     <t>Kevlar Epoxy</t>
   </si>
   <si>
-    <t>Glass Epoxy</t>
+    <t>Carbon Epoxy</t>
   </si>
   <si>
-    <t>Carbon Epoxy</t>
+    <t>Glass Epoxy</t>
   </si>
 </sst>
 </file>
@@ -409,10 +409,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>-15</v>
+        <v>-75</v>
       </c>
       <c r="D2">
-        <v>0.3087542249593882</v>
+        <v>0.1149964717329423</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -423,10 +423,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>-75</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0.1753928817353048</v>
+        <v>0.2117507750704913</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -440,7 +440,7 @@
         <v>45</v>
       </c>
       <c r="D4">
-        <v>0.1397850898685769</v>
+        <v>0.1637626273087146</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -451,10 +451,10 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>-75</v>
+        <v>60</v>
       </c>
       <c r="D5">
-        <v>0.1842232442254685</v>
+        <v>0.3225316272253315</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -462,13 +462,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>-90</v>
       </c>
       <c r="D6">
-        <v>0.1027043927184242</v>
+        <v>0.1567194869119664</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -476,13 +476,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="D7">
-        <v>0.200285264123941</v>
+        <v>0.1468255612575169</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -493,10 +493,10 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>-15</v>
+        <v>90</v>
       </c>
       <c r="D8">
-        <v>0.1306595211680086</v>
+        <v>0.1146116802397564</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -504,13 +504,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>-60</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.1012234495480952</v>
+        <v>0.1546749862494727</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -518,13 +518,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>15</v>
+        <v>-45</v>
       </c>
       <c r="D10">
-        <v>0.2891619568834529</v>
+        <v>0.3358321381769125</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -532,13 +532,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>90</v>
+        <v>-60</v>
       </c>
       <c r="D11">
-        <v>0.1287144423938974</v>
+        <v>0.3644997473517692</v>
       </c>
     </row>
   </sheetData>
@@ -548,7 +548,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -564,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>49196.03755215795</v>
+        <v>32884.81285385437</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>49196.03755215795</v>
+        <v>32884.81285385437</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -580,7 +580,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>45073.45378665238</v>
+        <v>32884.81285385437</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -588,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>45073.45378665238</v>
+        <v>32884.81285385437</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -596,7 +596,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>45073.45378665238</v>
+        <v>32884.81285385437</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -604,7 +604,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>41677.68714387548</v>
+        <v>32884.81285385437</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -612,7 +612,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>41677.68714387548</v>
+        <v>32617.37529622098</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -620,7 +620,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>41677.68714387548</v>
+        <v>32617.37529622098</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -628,7 +628,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>41677.68714387548</v>
+        <v>32138.74224230903</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -636,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>38871.30410537889</v>
+        <v>32138.74224230903</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -644,7 +644,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>35926.5862018168</v>
+        <v>29406.0720694309</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -652,7 +652,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>35926.5862018168</v>
+        <v>26557.72392211551</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -660,7 +660,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>35926.5862018168</v>
+        <v>26557.72392211551</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -668,7 +668,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>33489.80169424388</v>
+        <v>26557.72392211551</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -676,7 +676,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>31697.69815428225</v>
+        <v>26011.23603633032</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -684,7 +684,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>31697.69815428225</v>
+        <v>26011.23603633032</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -692,7 +692,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>31697.69815428225</v>
+        <v>26011.23603633032</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -700,7 +700,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>31697.69815428225</v>
+        <v>36200.619418008</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -708,7 +708,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -716,7 +716,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -724,7 +724,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -732,7 +732,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -740,7 +740,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -748,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -756,7 +756,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -764,7 +764,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -772,7 +772,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -780,7 +780,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -788,7 +788,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>31697.69815428225</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -796,7 +796,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -804,7 +804,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -812,7 +812,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -820,7 +820,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -828,7 +828,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -836,7 +836,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -844,7 +844,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -852,7 +852,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -860,7 +860,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -868,7 +868,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -876,7 +876,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -884,7 +884,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>28948.18546584623</v>
+        <v>30882.59219623895</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -892,7 +892,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -900,7 +900,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -908,7 +908,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -916,7 +916,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -924,7 +924,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -932,7 +932,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -940,7 +940,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -948,7 +948,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -956,7 +956,407 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>28948.18546584623</v>
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>28131.16935321542</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>29722.29662916494</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>29722.29662916494</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>29722.29662916494</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>29722.29662916494</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>29722.29662916494</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>30384.02657136974</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>30384.02657136974</v>
       </c>
     </row>
   </sheetData>
@@ -966,7 +1366,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -982,7 +1382,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>86.26334164279416</v>
+        <v>66.50686176212176</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -990,7 +1390,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>86.26334164279416</v>
+        <v>66.50686176212176</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -998,7 +1398,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>74.41514062751065</v>
+        <v>66.50686176212176</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1006,7 +1406,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>74.41514062751065</v>
+        <v>66.50686176212176</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1014,7 +1414,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>74.41514062751065</v>
+        <v>66.50686176212176</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1022,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>67.22376733831372</v>
+        <v>66.50686176212176</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1030,7 +1430,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>67.22376733831372</v>
+        <v>76.20119958389051</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1038,7 +1438,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>67.22376733831372</v>
+        <v>76.20119958389051</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1046,7 +1446,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>67.22376733831372</v>
+        <v>74.41233715329093</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1054,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>63.0998837767383</v>
+        <v>74.41233715329093</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1062,7 +1462,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>61.12074840832162</v>
+        <v>80.00916405331211</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1070,7 +1470,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>61.12074840832162</v>
+        <v>68.35614135784789</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1078,7 +1478,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>61.12074840832162</v>
+        <v>68.35614135784789</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1086,7 +1486,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>64.30331249968293</v>
+        <v>68.35614135784789</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1094,7 +1494,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>62.60929878125834</v>
+        <v>76.52675285670938</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1102,7 +1502,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>62.60929878125834</v>
+        <v>76.52675285670938</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1110,7 +1510,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>62.60929878125834</v>
+        <v>76.52675285670938</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1118,7 +1518,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>62.60929878125834</v>
+        <v>91.89172434903617</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1126,7 +1526,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1134,7 +1534,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1142,7 +1542,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1150,7 +1550,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1158,7 +1558,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1166,7 +1566,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1174,7 +1574,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1182,7 +1582,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1190,7 +1590,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1198,7 +1598,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1206,7 +1606,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>62.60929878125834</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1214,7 +1614,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1222,7 +1622,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1230,7 +1630,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1238,7 +1638,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1246,7 +1646,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1254,7 +1654,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1262,7 +1662,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1270,7 +1670,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1278,7 +1678,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -1286,7 +1686,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -1294,7 +1694,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1302,7 +1702,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>51.55185908270218</v>
+        <v>88.39158338344052</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -1310,7 +1710,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -1318,7 +1718,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -1326,7 +1726,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1334,7 +1734,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1342,7 +1742,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1350,7 +1750,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -1358,7 +1758,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -1366,7 +1766,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -1374,7 +1774,407 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>51.55185908270218</v>
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>73.3121480643116</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>84.80431302823527</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>84.80431302823527</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>84.80431302823527</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>84.80431302823527</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>84.80431302823527</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="1">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="1">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="1">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="1">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="1">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="1">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="1">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="1">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="1">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="1">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="1">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="1">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="1">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>80.63429180988251</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="1">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>80.63429180988251</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +2184,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1400,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>28948.18546584623</v>
+        <v>27584.63613476182</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1408,7 +2208,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>28948.18546584623</v>
+        <v>44859.82582068203</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1416,87 +2216,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>28948.18546584623</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>28948.18546584623</v>
+        <v>38204.26982196342</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +2226,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1522,7 +2242,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>51.55185908270218</v>
+        <v>57.09931918069268</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1530,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>51.55185908270218</v>
+        <v>48.82880849655801</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1538,87 +2258,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>51.55185908270218</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>51.55185908270218</v>
+        <v>50.86833364428222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>